<commit_message>
Comprobante PDF con Formulario y Logo por empresa
</commit_message>
<xml_diff>
--- a/Excels/PDF para hacer Fleet 15Mayo2023.xlsx
+++ b/Excels/PDF para hacer Fleet 15Mayo2023.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Flutter\fleetdeliveryapp\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8284DC7C-92BC-405B-8AAA-847627D3FD7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501C119F-EA3A-4C94-81F7-02F6489C1C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E730531F-D069-4803-819F-CF718A479D9C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>personall flow no va</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>contador</t>
+  </si>
+  <si>
+    <t>558 x 168</t>
   </si>
 </sst>
 </file>
@@ -527,9 +530,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{350F6290-3D44-4321-A6C1-F9C48C40A40B}">
-  <dimension ref="G1:O30"/>
+  <dimension ref="C1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -621,32 +626,37 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
       <c r="J20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.3">
       <c r="J22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
       <c r="J23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.3">
       <c r="J25" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.3">
       <c r="G27" t="s">
         <v>24</v>
       </c>
@@ -654,7 +664,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:10" x14ac:dyDescent="0.3">
       <c r="G28">
         <v>1</v>
       </c>
@@ -663,7 +673,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="29" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:10" x14ac:dyDescent="0.3">
       <c r="G29">
         <v>2</v>
       </c>
@@ -672,7 +682,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="30" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:10" x14ac:dyDescent="0.3">
       <c r="G30">
         <v>3</v>
       </c>

</xml_diff>